<commit_message>
[fix] Define functions to set phases, set trajectories and set values
</commit_message>
<xml_diff>
--- a/model/N2O_Properties.xlsx
+++ b/model/N2O_Properties.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Desktop\RockETS\Rocket\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Desktop\RockETS\Rockets\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F642C8-FE2C-4B0E-A7EB-F9039D0C779A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AE09EF-BA79-45DE-AF91-2F8CA005EFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <r>
       <rPr>
@@ -134,9 +134,6 @@
       </rPr>
       <t>[J/kg]</t>
     </r>
-  </si>
-  <si>
-    <t>#</t>
   </si>
 </sst>
 </file>
@@ -613,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -629,9 +626,10 @@
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
     <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -654,7 +652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>182.32999999999998</v>
       </c>
@@ -680,7 +678,7 @@
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>183.14999999999998</v>
       </c>
@@ -706,7 +704,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>184.69</v>
       </c>
@@ -732,7 +730,7 @@
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>188.14999999999998</v>
       </c>
@@ -758,7 +756,7 @@
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
     </row>
-    <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>193.14999999999998</v>
       </c>
@@ -784,7 +782,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
     </row>
-    <row r="7" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>198.14999999999998</v>
       </c>
@@ -809,11 +807,8 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="Q7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>203.14999999999998</v>
       </c>
@@ -839,7 +834,7 @@
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
     </row>
-    <row r="9" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>208.14999999999998</v>
       </c>
@@ -865,7 +860,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
     </row>
-    <row r="10" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>213.14999999999998</v>
       </c>
@@ -891,7 +886,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
     </row>
-    <row r="11" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>218.14999999999998</v>
       </c>
@@ -917,7 +912,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>223.14999999999998</v>
       </c>
@@ -943,7 +938,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
     </row>
-    <row r="13" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>228.14999999999998</v>
       </c>
@@ -969,7 +964,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>233.14999999999998</v>
       </c>
@@ -995,7 +990,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
     </row>
-    <row r="15" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>238.14999999999998</v>
       </c>
@@ -1021,7 +1016,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>243.14999999999998</v>
       </c>
@@ -1418,6 +1413,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="db291fd8-3cfd-4be4-91ca-3fbeb332f44f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8e871639-4d03-4815-a297-7bb177073573">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010002D6281A9682AF4A98F873C035B5E8DC" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="282a728d77070331ab7eb8d7a35c54d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8e871639-4d03-4815-a297-7bb177073573" xmlns:ns3="db291fd8-3cfd-4be4-91ca-3fbeb332f44f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="988ca22d43628ba535d429bd9e26d0be" ns2:_="" ns3:_="">
     <xsd:import namespace="8e871639-4d03-4815-a297-7bb177073573"/>
@@ -1660,17 +1666,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="db291fd8-3cfd-4be4-91ca-3fbeb332f44f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8e871639-4d03-4815-a297-7bb177073573">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1681,6 +1676,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2C330A-B4AB-461D-A1A7-AF2BB71633F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="db291fd8-3cfd-4be4-91ca-3fbeb332f44f"/>
+    <ds:schemaRef ds:uri="8e871639-4d03-4815-a297-7bb177073573"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E34B677-0C62-4709-9ED2-D921F0DD1944}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1699,17 +1705,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2C330A-B4AB-461D-A1A7-AF2BB71633F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="db291fd8-3cfd-4be4-91ca-3fbeb332f44f"/>
-    <ds:schemaRef ds:uri="8e871639-4d03-4815-a297-7bb177073573"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27AC8AC7-74CA-4DED-BB6F-357BDD77ABC5}">
   <ds:schemaRefs>

</xml_diff>